<commit_message>
#1 Teacher dashboard - Removed few columns from the PROGRESS tab table
#2 Student dashboard - UI changes to teh question display page
</commit_message>
<xml_diff>
--- a/Documents/QuestionBank/7/AlgebraicExpressions.xlsx
+++ b/Documents/QuestionBank/7/AlgebraicExpressions.xlsx
@@ -2160,8 +2160,8 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>